<commit_message>
R2D/R2U data removed in Data3
</commit_message>
<xml_diff>
--- a/Data_list.xlsx
+++ b/Data_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comic\Desktop\CircuitFault_Detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE716307-6E3E-49A0-A1CC-346F3A5B0EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E38E4F-06B1-4D82-959F-DEE18FB440B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="-10020" windowWidth="21840" windowHeight="38040" xr2:uid="{E0F49974-8A92-4DF3-94D5-4F0151BC6DE9}"/>
   </bookViews>
@@ -598,7 +598,7 @@
   <dimension ref="A1:K75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="K84" sqref="K84"/>
+      <selection activeCell="M56" sqref="M56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -649,7 +649,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:11" hidden="1">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -695,7 +695,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:11" hidden="1">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -718,7 +718,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1">
+    <row r="5" spans="1:11">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -744,7 +744,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="3" customFormat="1" hidden="1">
+    <row r="6" spans="1:11" s="3" customFormat="1">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -793,7 +793,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:11" hidden="1">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -819,7 +819,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -868,7 +868,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -894,7 +894,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="3" customFormat="1" hidden="1">
+    <row r="12" spans="1:11" s="3" customFormat="1">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:11" hidden="1">
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:11" hidden="1">
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:11" hidden="1">
+    <row r="26" spans="1:11">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -1293,7 +1293,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="3" customFormat="1" hidden="1">
+    <row r="27" spans="1:11" s="3" customFormat="1">
       <c r="A27" s="3" t="s">
         <v>21</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:11" hidden="1">
+    <row r="28" spans="1:11">
       <c r="A28" t="s">
         <v>23</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:11" hidden="1">
+    <row r="30" spans="1:11">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:11" hidden="1">
+    <row r="31" spans="1:11">
       <c r="A31" t="s">
         <v>23</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="3" customFormat="1" hidden="1">
+    <row r="32" spans="1:11" s="3" customFormat="1">
       <c r="A32" s="3" t="s">
         <v>23</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:11" hidden="1">
+    <row r="33" spans="1:11">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:11" hidden="1">
+    <row r="35" spans="1:11">
       <c r="A35" t="s">
         <v>25</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:11" s="3" customFormat="1" hidden="1">
+    <row r="36" spans="1:11" s="3" customFormat="1">
       <c r="A36" s="3" t="s">
         <v>25</v>
       </c>
@@ -1585,11 +1585,11 @@
       <c r="I37" t="s">
         <v>7</v>
       </c>
-      <c r="K37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11">
+      <c r="J37" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" hidden="1">
       <c r="A38" t="s">
         <v>28</v>
       </c>
@@ -1611,8 +1611,8 @@
       <c r="I38" t="s">
         <v>9</v>
       </c>
-      <c r="K38" t="s">
-        <v>9</v>
+      <c r="J38" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="39" spans="1:11" hidden="1">
@@ -1637,8 +1637,8 @@
       <c r="I39" t="s">
         <v>7</v>
       </c>
-      <c r="K39" t="s">
-        <v>7</v>
+      <c r="J39" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:11" s="3" customFormat="1" hidden="1">
@@ -1663,8 +1663,8 @@
       <c r="I40" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K40" s="3" t="s">
-        <v>7</v>
+      <c r="J40" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:11" hidden="1">
@@ -1689,11 +1689,11 @@
       <c r="I41" t="s">
         <v>7</v>
       </c>
-      <c r="K41" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11">
+      <c r="J41" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" hidden="1">
       <c r="A42" t="s">
         <v>30</v>
       </c>
@@ -1715,8 +1715,8 @@
       <c r="I42" t="s">
         <v>9</v>
       </c>
-      <c r="K42" t="s">
-        <v>9</v>
+      <c r="J42" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="43" spans="1:11" hidden="1">
@@ -1743,9 +1743,10 @@
       <c r="I43" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K43" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="J43" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K43" s="2"/>
     </row>
     <row r="44" spans="1:11" s="3" customFormat="1" hidden="1">
       <c r="A44" s="3" t="s">
@@ -1769,8 +1770,8 @@
       <c r="I44" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K44" s="3" t="s">
-        <v>7</v>
+      <c r="J44" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:11" hidden="1">
@@ -1799,7 +1800,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:11" hidden="1">
+    <row r="46" spans="1:11">
       <c r="A46" t="s">
         <v>32</v>
       </c>
@@ -1825,7 +1826,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:11" hidden="1">
+    <row r="47" spans="1:11">
       <c r="A47" s="2" t="s">
         <v>32</v>
       </c>
@@ -1881,7 +1882,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:11" hidden="1">
+    <row r="49" spans="1:11">
       <c r="A49" s="2" t="s">
         <v>32</v>
       </c>
@@ -1909,7 +1910,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:11" s="3" customFormat="1" hidden="1">
+    <row r="50" spans="1:11" s="3" customFormat="1">
       <c r="A50" s="3" t="s">
         <v>32</v>
       </c>
@@ -2068,7 +2069,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:11" hidden="1">
+    <row r="56" spans="1:11">
       <c r="A56" s="2" t="s">
         <v>34</v>
       </c>
@@ -2096,7 +2097,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:11" hidden="1">
+    <row r="57" spans="1:11">
       <c r="A57" s="2" t="s">
         <v>34</v>
       </c>
@@ -2150,7 +2151,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:11" hidden="1">
+    <row r="59" spans="1:11">
       <c r="A59" s="2" t="s">
         <v>34</v>
       </c>
@@ -2178,7 +2179,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:11" s="3" customFormat="1" hidden="1">
+    <row r="60" spans="1:11" s="3" customFormat="1">
       <c r="A60" s="3" t="s">
         <v>34</v>
       </c>
@@ -2259,7 +2260,7 @@
       </c>
       <c r="K62" s="2"/>
     </row>
-    <row r="63" spans="1:11" hidden="1">
+    <row r="63" spans="1:11">
       <c r="A63" s="2" t="s">
         <v>36</v>
       </c>
@@ -2287,7 +2288,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:11" hidden="1">
+    <row r="64" spans="1:11">
       <c r="A64" s="2" t="s">
         <v>36</v>
       </c>
@@ -2343,7 +2344,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:11" hidden="1">
+    <row r="66" spans="1:11">
       <c r="A66" s="2" t="s">
         <v>36</v>
       </c>
@@ -2399,7 +2400,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:11" s="3" customFormat="1" hidden="1">
+    <row r="68" spans="1:11" s="3" customFormat="1">
       <c r="A68" s="3" t="s">
         <v>36</v>
       </c>
@@ -2477,7 +2478,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="71" spans="1:11" hidden="1">
+    <row r="71" spans="1:11">
       <c r="A71" t="s">
         <v>38</v>
       </c>
@@ -2503,7 +2504,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:11" hidden="1">
+    <row r="72" spans="1:11">
       <c r="A72" t="s">
         <v>38</v>
       </c>
@@ -2555,7 +2556,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:11" hidden="1">
+    <row r="74" spans="1:11">
       <c r="A74" t="s">
         <v>38</v>
       </c>
@@ -2581,7 +2582,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:11" s="3" customFormat="1" hidden="1">
+    <row r="75" spans="1:11" s="3" customFormat="1">
       <c r="A75" s="3" t="s">
         <v>38</v>
       </c>
@@ -2610,9 +2611,9 @@
   </sheetData>
   <autoFilter ref="A1:K75" xr:uid="{530C5BE1-32B8-4EDB-B92A-6F0CE81EF3CC}">
     <filterColumn colId="10">
-      <filters>
-        <filter val="Test"/>
-      </filters>
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
     </filterColumn>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>